<commit_message>
Add CBO e faz ajustes nas pages de MI e MC
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-BRDose.xlsx
+++ b/docs/CodeSystem-BRDose.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="286">
   <si>
     <t>Property</t>
   </si>
@@ -141,490 +141,736 @@
     <t>1ª Dose</t>
   </si>
   <si>
+    <t>D1</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
     <t>2ª Dose</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
     <t>3ª Dose</t>
   </si>
   <si>
+    <t>D3</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
     <t>4ª Dose</t>
   </si>
   <si>
+    <t>D4</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
     <t>5ª Dose</t>
   </si>
   <si>
+    <t>D5</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>1º Reforço</t>
   </si>
   <si>
+    <t>R1</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
     <t>2º Reforço</t>
   </si>
   <si>
+    <t>R2</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
     <t>Dose</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
     <t>Única</t>
   </si>
   <si>
+    <t>DU</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
     <t>Revacinação</t>
   </si>
   <si>
+    <t>REV</t>
+  </si>
+  <si>
     <t>11</t>
   </si>
   <si>
     <t>Tratamento com uma dose</t>
   </si>
   <si>
+    <t>T1</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
     <t>Tratamento com duas doses</t>
   </si>
   <si>
+    <t>T2</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
     <t>Tratamento com três doses</t>
   </si>
   <si>
+    <t>T3</t>
+  </si>
+  <si>
     <t>14</t>
   </si>
   <si>
     <t>Tratamento com quatro doses</t>
   </si>
   <si>
+    <t>T4</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
     <t>Tratamento com cinco doses</t>
   </si>
   <si>
+    <t>T5</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
     <t>Tratamento com seis doses</t>
   </si>
   <si>
+    <t>T6</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
     <t>Tratamento com sete doses</t>
   </si>
   <si>
+    <t>T7</t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
     <t>Tratamento com oito doses</t>
   </si>
   <si>
+    <t>T8</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
     <t>Tratamento com nove doses</t>
   </si>
   <si>
+    <t>T9</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
     <t>Tratamento com dez doses</t>
   </si>
   <si>
+    <t>T10</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
     <t>Tratamento com onze doses</t>
   </si>
   <si>
+    <t>T11</t>
+  </si>
+  <si>
     <t>22</t>
   </si>
   <si>
     <t>Tratamento com doze doses</t>
   </si>
   <si>
+    <t>T12</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
     <t>Tratamento com treze doses</t>
   </si>
   <si>
+    <t>T13</t>
+  </si>
+  <si>
     <t>24</t>
   </si>
   <si>
     <t>Tratamento com quartorze doses</t>
   </si>
   <si>
+    <t>T14</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
     <t>Tratamento com quinze doses</t>
   </si>
   <si>
+    <t>T15</t>
+  </si>
+  <si>
     <t>26</t>
   </si>
   <si>
     <t>Tratamento com dezesseis doses</t>
   </si>
   <si>
+    <t>T16</t>
+  </si>
+  <si>
     <t>27</t>
   </si>
   <si>
     <t>Tratamento com dezessete doses</t>
   </si>
   <si>
+    <t>T17</t>
+  </si>
+  <si>
     <t>28</t>
   </si>
   <si>
     <t>Tratamento com dezoito doses</t>
   </si>
   <si>
+    <t>T18</t>
+  </si>
+  <si>
     <t>29</t>
   </si>
   <si>
     <t>Tratamento com dezenove doses</t>
   </si>
   <si>
+    <t>T19</t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
     <t>Tratamento com vinte doses</t>
   </si>
   <si>
+    <t>T20</t>
+  </si>
+  <si>
     <t>31</t>
   </si>
   <si>
     <t>Tratamento com vinte e quatro doses</t>
   </si>
   <si>
+    <t>T24</t>
+  </si>
+  <si>
     <t>32</t>
   </si>
   <si>
     <t>1ª Dose Revacinação</t>
   </si>
   <si>
+    <t>D1REV</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
     <t>2ª Dose Revacinação</t>
   </si>
   <si>
+    <t>D2REV</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
     <t>3ª Dose Revacinação</t>
   </si>
   <si>
+    <t>D3REV</t>
+  </si>
+  <si>
     <t>35</t>
   </si>
   <si>
     <t>4ª Dose Revacinação</t>
   </si>
   <si>
+    <t>D4REV</t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
     <t>Dose Inicial</t>
   </si>
   <si>
+    <t>DI</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
     <t>Dose Adicional</t>
   </si>
   <si>
+    <t>DA</t>
+  </si>
+  <si>
     <t>38</t>
   </si>
   <si>
     <t>Reforço</t>
   </si>
   <si>
+    <t>REF</t>
+  </si>
+  <si>
     <t>39</t>
   </si>
   <si>
     <t>3º Reforço</t>
   </si>
   <si>
+    <t>R3</t>
+  </si>
+  <si>
     <t>40</t>
   </si>
   <si>
     <t>4º Reforço</t>
   </si>
   <si>
+    <t>R4</t>
+  </si>
+  <si>
     <t>41</t>
   </si>
   <si>
     <t>5º Reforço</t>
   </si>
   <si>
+    <t>R5</t>
+  </si>
+  <si>
     <t>42</t>
   </si>
   <si>
     <t>6º Reforço</t>
   </si>
   <si>
+    <t>R6</t>
+  </si>
+  <si>
     <t>43</t>
   </si>
   <si>
     <t>5ª Dose Revacinação</t>
   </si>
   <si>
+    <t>D5REV</t>
+  </si>
+  <si>
     <t>44</t>
   </si>
   <si>
     <t>1ª Dose Fracionada</t>
   </si>
   <si>
+    <t>D1F</t>
+  </si>
+  <si>
     <t>45</t>
   </si>
   <si>
     <t>2ª Dose Fracionada</t>
   </si>
   <si>
+    <t>D2F</t>
+  </si>
+  <si>
     <t>46</t>
   </si>
   <si>
     <t>3ª Dose Fracionada</t>
   </si>
   <si>
+    <t>D3F</t>
+  </si>
+  <si>
     <t>47</t>
   </si>
   <si>
     <t>4ª Dose Fracionada</t>
   </si>
   <si>
+    <t>D4F</t>
+  </si>
+  <si>
     <t>48</t>
   </si>
   <si>
     <t>5ª Dose Fracionada</t>
   </si>
   <si>
+    <t>D5F</t>
+  </si>
+  <si>
     <t>49</t>
   </si>
   <si>
     <t>1ª Dose Dobrada</t>
   </si>
   <si>
+    <t>D1D</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
     <t>2ª Dose Dobrada</t>
   </si>
   <si>
+    <t>D2D</t>
+  </si>
+  <si>
     <t>51</t>
   </si>
   <si>
     <t>3ª Dose Dobrada</t>
   </si>
   <si>
+    <t>D3D</t>
+  </si>
+  <si>
     <t>52</t>
   </si>
   <si>
     <t>4ª Dose Dobrada</t>
   </si>
   <si>
+    <t>D4D</t>
+  </si>
+  <si>
     <t>53</t>
   </si>
   <si>
     <t>1ª Dose Revacinação Dobrada</t>
   </si>
   <si>
+    <t>D1REVD</t>
+  </si>
+  <si>
     <t>54</t>
   </si>
   <si>
     <t>2ª Dose Revacinação Dobrada</t>
   </si>
   <si>
+    <t>D2REVD</t>
+  </si>
+  <si>
     <t>55</t>
   </si>
   <si>
     <t>3ª Dose Revacinação Dobrada</t>
   </si>
   <si>
+    <t>D3REVD</t>
+  </si>
+  <si>
     <t>56</t>
   </si>
   <si>
     <t>4ª Dose Revacinação Dobrada</t>
   </si>
   <si>
+    <t>D4REVD</t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
     <t>Dose Zero</t>
   </si>
   <si>
+    <t>D0</t>
+  </si>
+  <si>
     <t>58</t>
   </si>
   <si>
     <t>Reforço Zero</t>
   </si>
   <si>
+    <t>R0</t>
+  </si>
+  <si>
     <t>59</t>
   </si>
   <si>
-    <t>Profilaxia com 1 frasco-ampola/ampola</t>
+    <t>Profilaxia/Tratamento com 1 frasco-ampola/ampola</t>
+  </si>
+  <si>
+    <t>P/T1</t>
   </si>
   <si>
     <t>60</t>
   </si>
   <si>
-    <t>Profilaxia com 2 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 2 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T2</t>
   </si>
   <si>
     <t>61</t>
   </si>
   <si>
-    <t>Profilaxia com 3 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 3 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T3</t>
   </si>
   <si>
     <t>62</t>
   </si>
   <si>
-    <t>Profilaxia com 4 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 4 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T4</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
-    <t>Profilaxia com 5 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 5 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T5</t>
   </si>
   <si>
     <t>64</t>
   </si>
   <si>
-    <t>Profilaxia com 6 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 6 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T6</t>
   </si>
   <si>
     <t>65</t>
   </si>
   <si>
-    <t>Profilaxia com 7 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 7 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T7</t>
   </si>
   <si>
     <t>66</t>
   </si>
   <si>
-    <t>Profilaxia com 8 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 8 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T8</t>
   </si>
   <si>
     <t>67</t>
   </si>
   <si>
-    <t>Profilaxia com 9 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 9 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T9</t>
   </si>
   <si>
     <t>68</t>
   </si>
   <si>
-    <t>Profilaxia com 10 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 10 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T10</t>
   </si>
   <si>
     <t>69</t>
   </si>
   <si>
-    <t>Profilaxia com 11 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 11 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T11</t>
   </si>
   <si>
     <t>70</t>
   </si>
   <si>
-    <t>Profilaxia com 12 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 12 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T12</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t>Profilaxia com 13 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 13 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T13</t>
   </si>
   <si>
     <t>72</t>
   </si>
   <si>
-    <t>Profilaxia com 14 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 14 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T14</t>
   </si>
   <si>
     <t>73</t>
   </si>
   <si>
-    <t>Profilaxia com 15 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 15 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T15</t>
   </si>
   <si>
     <t>74</t>
   </si>
   <si>
-    <t>Profilaxia com 16 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 16 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T16</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
-    <t>Profilaxia com 17 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 17 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T17</t>
   </si>
   <si>
     <t>76</t>
   </si>
   <si>
-    <t>Profilaxia com 18 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 18 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T18</t>
   </si>
   <si>
     <t>77</t>
   </si>
   <si>
-    <t>Profilaxia com 19 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 19 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T19</t>
   </si>
   <si>
     <t>78</t>
   </si>
   <si>
-    <t>Profilaxia com 20 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 20 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T20</t>
   </si>
   <si>
     <t>79</t>
   </si>
   <si>
-    <t>Profilaxia com 21 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 21 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T21</t>
   </si>
   <si>
     <t>80</t>
   </si>
   <si>
-    <t>Profilaxia com 22 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 22 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T22</t>
   </si>
   <si>
     <t>81</t>
   </si>
   <si>
-    <t>Profilaxia com 23 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 23 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T23</t>
   </si>
   <si>
     <t>82</t>
   </si>
   <si>
-    <t>Profilaxia com 24 frascos-ampolas/ampolas</t>
+    <t>Profilaxia/Tratamento com 24 frascos-ampolas/ampolas</t>
+  </si>
+  <si>
+    <t>P/T24</t>
   </si>
 </sst>
 </file>
@@ -965,979 +1211,1143 @@
       <c r="C2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>42</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>45</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>51</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>54</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>57</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>60</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>63</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>69</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>72</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>96</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>102</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>105</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>108</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>111</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>114</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>117</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="D28" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>120</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>123</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>126</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="D31" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>129</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="D32" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>132</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="D33" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="D33" t="s" s="2">
+        <v>135</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="D34" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>138</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>141</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="D36" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="D36" t="s" s="2">
+        <v>144</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>147</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="D38" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="D38" t="s" s="2">
+        <v>150</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="D39" s="2"/>
+        <v>152</v>
+      </c>
+      <c r="D39" t="s" s="2">
+        <v>153</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="D40" t="s" s="2">
+        <v>156</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="D41" t="s" s="2">
+        <v>159</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="D42" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="D42" t="s" s="2">
+        <v>162</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="D43" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="D43" t="s" s="2">
+        <v>165</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="D44" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="D44" t="s" s="2">
+        <v>168</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>171</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="D46" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="D46" t="s" s="2">
+        <v>174</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="D47" t="s" s="2">
+        <v>177</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="D48" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="D48" t="s" s="2">
+        <v>180</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D49" t="s" s="2">
+        <v>183</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="D50" s="2"/>
+        <v>185</v>
+      </c>
+      <c r="D50" t="s" s="2">
+        <v>186</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="D51" t="s" s="2">
+        <v>189</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="D52" s="2"/>
+        <v>191</v>
+      </c>
+      <c r="D52" t="s" s="2">
+        <v>192</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="D53" t="s" s="2">
+        <v>195</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="D54" s="2"/>
+        <v>197</v>
+      </c>
+      <c r="D54" t="s" s="2">
+        <v>198</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>146</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="D55" t="s" s="2">
+        <v>201</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>148</v>
+        <v>202</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="D56" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="D56" t="s" s="2">
+        <v>204</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="D57" t="s" s="2">
+        <v>207</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>209</v>
+      </c>
+      <c r="D58" t="s" s="2">
+        <v>210</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="D59" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="D59" t="s" s="2">
+        <v>213</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="D60" s="2"/>
+        <v>215</v>
+      </c>
+      <c r="D60" t="s" s="2">
+        <v>216</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>158</v>
+        <v>217</v>
       </c>
       <c r="C61" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="D61" s="2"/>
+        <v>218</v>
+      </c>
+      <c r="D61" t="s" s="2">
+        <v>219</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="D62" t="s" s="2">
+        <v>222</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D63" t="s" s="2">
+        <v>225</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>164</v>
+        <v>226</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>227</v>
+      </c>
+      <c r="D64" t="s" s="2">
+        <v>228</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>166</v>
+        <v>229</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>230</v>
+      </c>
+      <c r="D65" t="s" s="2">
+        <v>231</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>168</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>233</v>
+      </c>
+      <c r="D66" t="s" s="2">
+        <v>234</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="C67" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="D67" s="2"/>
+        <v>236</v>
+      </c>
+      <c r="D67" t="s" s="2">
+        <v>237</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>172</v>
+        <v>238</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="D68" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="D68" t="s" s="2">
+        <v>240</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>174</v>
+        <v>241</v>
       </c>
       <c r="C69" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>242</v>
+      </c>
+      <c r="D69" t="s" s="2">
+        <v>243</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="C70" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>245</v>
+      </c>
+      <c r="D70" t="s" s="2">
+        <v>246</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="D71" t="s" s="2">
+        <v>249</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="C72" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="D72" s="2"/>
+        <v>251</v>
+      </c>
+      <c r="D72" t="s" s="2">
+        <v>252</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>182</v>
+        <v>253</v>
       </c>
       <c r="C73" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="D73" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="D73" t="s" s="2">
+        <v>255</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>184</v>
+        <v>256</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="D74" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="D74" t="s" s="2">
+        <v>258</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>186</v>
+        <v>259</v>
       </c>
       <c r="C75" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="D75" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="D75" t="s" s="2">
+        <v>261</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>188</v>
+        <v>262</v>
       </c>
       <c r="C76" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="D76" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="D76" t="s" s="2">
+        <v>264</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>190</v>
+        <v>265</v>
       </c>
       <c r="C77" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="D77" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="D77" t="s" s="2">
+        <v>267</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>192</v>
+        <v>268</v>
       </c>
       <c r="C78" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>269</v>
+      </c>
+      <c r="D78" t="s" s="2">
+        <v>270</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>194</v>
+        <v>271</v>
       </c>
       <c r="C79" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="D79" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="D79" t="s" s="2">
+        <v>273</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>196</v>
+        <v>274</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="D80" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="D80" t="s" s="2">
+        <v>276</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>198</v>
+        <v>277</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="D81" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="D81" t="s" s="2">
+        <v>279</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="C82" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="D82" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="D82" t="s" s="2">
+        <v>282</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
         <v>40</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>202</v>
+        <v>283</v>
       </c>
       <c r="C83" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="D83" s="2"/>
+        <v>284</v>
+      </c>
+      <c r="D83" t="s" s="2">
+        <v>285</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>